<commit_message>
AIP-1382 AIP-1322 Changes made to check for variable voltage range with 50 retry attempts
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/FR_DISPATCHRMS_DATASET_9Channel/1U3I3I_phB.xlsx
+++ b/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/FR_DISPATCHRMS_DATASET_9Channel/1U3I3I_phB.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6727D6-4DEF-4B88-9D12-48520E6CB92E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA624625-5256-4515-A94B-7DDFCE5331B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -1352,8 +1352,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,7 +1550,7 @@
         <v>96</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1699,7 +1699,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>